<commit_message>
Revert "Merge branch 'main' of https://github.com/hyungtak/NGP_2020_2 into main"
This reverts commit 4fa5c42ae54d24ccefc0701fa6ee3f97bef45b23, reversing
changes made to acddcf1ecd5dfe67655989a84c776de6d6302b71.
</commit_message>
<xml_diff>
--- a/일정관리표.xlsx
+++ b/일정관리표.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FE2DCF-5E0D-4742-8E61-C06455D75071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E8871E-C6EF-4D1B-8D5C-2611C3F1D77C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="110">
   <si>
     <t>월</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -277,6 +277,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>방향키입력 처리 구현
+폭탄은 나중에 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>제대로 작동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -355,6 +360,16 @@
   <si>
     <t>불길 삭제가 안됨
 불길 타이머도 관리 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충돌처리 제작,
+SceneData는 나중에</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폭탄 타이머 및 
+폭탄 구조체 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -369,6 +384,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">Lobby thread 구현중.
+아직 제대로 작동 안됨
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Renderer()수정 필요 없음
 폭탄 불길 처리 구현 덜함</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -378,6 +399,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>매칭 테스트 성공.
+다만 대기 씬이 없기에 추가 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>서버시간 사용하여 폭탄 불길 처리완료.
 폭탄은 이제 끝</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -387,8 +413,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>게임 시작 화면 구현.
+종료는 나중으로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>매칭중/게임중 보내주는
  데이터 구분 구현 완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 
+사망 처리 구현중</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -424,6 +460,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>SendToServer() 수정 성공.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>게임 테스트 성공</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -441,6 +481,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>branch merge 오류 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>해결법</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -454,131 +498,6 @@
   </si>
   <si>
     <t>채택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 시작 화면 구현.
-종료는 12/04일전까지
-구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매칭 테스트 성공.
-다만 대기 씬이 없기에 
-12/01일까지 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lobby thread 구현중.
-아직 제대로 작동 안됨
-12/01까지 구현 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플레이어 
-사망 처리 구현중
-12/04일까지 구현필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방향키입력 처리 구현
-폭탄은 11/20일까지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>폭탄키 입력 처리 완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대기씬 구현 완료
-다만 너무 밋밋해서 추가 수정 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">폭탄 타이머 및 
-폭탄 구조체 수정
-아이템구현은 원휘재,
-11/27일 전까지 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>충돌처리 제작,
-SceneData는 11/29전까지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SceneData 수정 완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateGameThread() 
-구현 성공
-SendToServer() 수정 성공.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>branch merge 오류 수정
-LobbyScene 이미지 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구현은 이전에 완료되었기에
-기존 PlayerData 수정을 함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플레이어 사망처리 구현완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 종료 조건 구현 완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>종료 씬 제작
-Renderer 수정
-Shader수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 종료 및 
-승리한 플레이어 
-출력 완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 테스트 중 
-게임이 끝나도 
-서버가 종료되지 않는 
-문제 발생</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트 성공</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 종료시
- 서버 종료 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Client 구조체 및 
-불필요한 코드 정리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>서버 구조체 및 
-불필요한 코드 정리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최종 테스트
-성공</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LowLevel 수정 및 정리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -589,7 +508,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,32 +531,8 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,23 +581,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -799,40 +679,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -915,143 +766,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="나쁨" xfId="2" builtinId="27"/>
-    <cellStyle name="보통" xfId="3" builtinId="28"/>
-    <cellStyle name="좋음" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1395,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:E41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1466,16 +1215,16 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="37" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1486,14 +1235,14 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="29" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="55"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1502,26 +1251,26 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="29" t="s">
+      <c r="E5" s="37"/>
+      <c r="F5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="55"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
@@ -1531,10 +1280,10 @@
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="31" t="s">
         <v>62</v>
       </c>
       <c r="H7" s="21"/>
@@ -1547,8 +1296,8 @@
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
       <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1559,8 +1308,8 @@
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1603,25 +1352,25 @@
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="55" t="s">
+      <c r="H12" s="37" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1629,84 +1378,84 @@
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="55"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="29" t="s">
+      <c r="F14" s="37"/>
+      <c r="G14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="55"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="48"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
+      <c r="C16" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>75</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="33" x14ac:dyDescent="0.3">
@@ -1714,22 +1463,24 @@
         <v>13</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1741,30 +1492,26 @@
         <v>62</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-    </row>
-    <row r="19" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="23"/>
       <c r="B19" s="5"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
-      <c r="E19" s="29" t="s">
-        <v>106</v>
-      </c>
+      <c r="E19" s="23"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="34" t="s">
-        <v>74</v>
-      </c>
+      <c r="G19" s="25"/>
       <c r="H19" s="23"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1797,25 +1544,25 @@
       <c r="A21" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="49" t="s">
+      <c r="H21" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1823,155 +1570,151 @@
       <c r="A22" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="32" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="29" t="s">
+      <c r="D22" s="32"/>
+      <c r="E22" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="54"/>
-      <c r="G22" s="32" t="s">
+      <c r="F22" s="33"/>
+      <c r="G22" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="50"/>
+      <c r="H22" s="32"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="29" t="s">
+      <c r="B23" s="33"/>
+      <c r="C23" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="32" t="s">
+      <c r="D23" s="33"/>
+      <c r="E23" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="51"/>
+      <c r="H23" s="33"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="48"/>
-    </row>
-    <row r="25" spans="1:10" ht="66" x14ac:dyDescent="0.3">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+    </row>
+    <row r="25" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="52" t="s">
-        <v>80</v>
+      <c r="B25" s="34" t="s">
+        <v>81</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="39" t="s">
-        <v>85</v>
+      <c r="D25" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>90</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="33" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="50"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>110</v>
+        <v>82</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>18</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H26" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="H26" s="31" t="s">
         <v>18</v>
       </c>
       <c r="I26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="51"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="36" t="s">
-        <v>18</v>
-      </c>
+      <c r="D27" s="33"/>
       <c r="E27" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="H27" s="51"/>
+        <v>93</v>
+      </c>
+      <c r="H27" s="33"/>
       <c r="I27" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="25"/>
       <c r="C28" s="23"/>
       <c r="D28" s="25"/>
       <c r="E28" s="24"/>
       <c r="F28" s="23"/>
-      <c r="G28" s="34" t="s">
-        <v>107</v>
-      </c>
+      <c r="G28" s="23"/>
       <c r="H28" s="25"/>
       <c r="I28" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2000,115 +1743,111 @@
         <v>44171</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="45" t="s">
+      <c r="F30" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="63" t="s">
+      <c r="G30" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="H30" s="49" t="s">
+      <c r="H30" s="31" t="s">
         <v>18</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="61"/>
-      <c r="E31" s="35" t="s">
+      <c r="D31" s="35"/>
+      <c r="E31" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="45" t="s">
+      <c r="F31" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="64"/>
-      <c r="H31" s="50"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="62"/>
-      <c r="E32" s="35" t="s">
+      <c r="D32" s="36"/>
+      <c r="E32" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="F32" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="65"/>
-      <c r="H32" s="51"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="48"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
     </row>
     <row r="34" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="E34" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="F34" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="G34" s="42" t="s">
-        <v>117</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
@@ -2116,23 +1855,17 @@
         <v>13</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>111</v>
+        <v>99</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F35" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="G35" s="52" t="s">
-        <v>118</v>
-      </c>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="22"/>
     </row>
     <row r="36" spans="1:10" ht="66" x14ac:dyDescent="0.3">
@@ -2140,21 +1873,17 @@
         <v>14</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="G36" s="51"/>
+        <v>100</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="22"/>
       <c r="H36" s="22"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -2191,16 +1920,16 @@
       <c r="A39" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="69" t="s">
+      <c r="C39" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="69" t="s">
+      <c r="D39" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E39" s="52" t="s">
+      <c r="E39" s="34" t="s">
         <v>15</v>
       </c>
       <c r="F39" s="21"/>
@@ -2211,10 +1940,10 @@
       <c r="A40" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="70"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="61"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
@@ -2223,99 +1952,46 @@
       <c r="A41" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="62"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
       <c r="H41" s="21"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="48"/>
-    </row>
-    <row r="43" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A43" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" s="67" t="s">
-        <v>119</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A44" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="66" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A45" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="66"/>
-    </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J48" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A42:H42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="G16:G18"/>
+  <mergeCells count="27">
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A6:H6"/>
     <mergeCell ref="D39:D41"/>
     <mergeCell ref="E39:E41"/>
     <mergeCell ref="G30:G32"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A6:H6"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A33:H33"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="F21:F22"/>
+    <mergeCell ref="H30:H32"/>
     <mergeCell ref="H21:H23"/>
     <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="D26:D27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>